<commit_message>
Unify MADEX API and implement canonical calculator
</commit_message>
<xml_diff>
--- a/extended_outcome/extended_scenario_results.xlsx
+++ b/extended_outcome/extended_scenario_results.xlsx
@@ -508,10 +508,10 @@
         <v>11.17</v>
       </c>
       <c r="I2" t="n">
-        <v>62.13</v>
+        <v>92.78</v>
       </c>
       <c r="J2" t="n">
-        <v>7.88</v>
+        <v>9.630000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -542,10 +542,10 @@
         <v>11.17</v>
       </c>
       <c r="I3" t="n">
-        <v>286.31</v>
+        <v>171.28</v>
       </c>
       <c r="J3" t="n">
-        <v>16.92</v>
+        <v>13.09</v>
       </c>
     </row>
     <row r="4">
@@ -576,10 +576,10 @@
         <v>17.51</v>
       </c>
       <c r="I4" t="n">
-        <v>84.98</v>
+        <v>171.31</v>
       </c>
       <c r="J4" t="n">
-        <v>9.220000000000001</v>
+        <v>13.09</v>
       </c>
     </row>
     <row r="5">
@@ -610,10 +610,10 @@
         <v>17.51</v>
       </c>
       <c r="I5" t="n">
-        <v>1917.02</v>
+        <v>600.1799999999999</v>
       </c>
       <c r="J5" t="n">
-        <v>43.78</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="6">
@@ -644,10 +644,10 @@
         <v>9.779999999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>72.42</v>
+        <v>83.16</v>
       </c>
       <c r="J6" t="n">
-        <v>8.51</v>
+        <v>9.119999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -678,10 +678,10 @@
         <v>9.779999999999999</v>
       </c>
       <c r="I7" t="n">
-        <v>156.57</v>
+        <v>113.81</v>
       </c>
       <c r="J7" t="n">
-        <v>12.51</v>
+        <v>10.67</v>
       </c>
     </row>
     <row r="8">
@@ -712,10 +712,10 @@
         <v>7.5</v>
       </c>
       <c r="I8" t="n">
-        <v>59.44</v>
+        <v>57.28</v>
       </c>
       <c r="J8" t="n">
-        <v>7.71</v>
+        <v>7.57</v>
       </c>
     </row>
     <row r="9">
@@ -746,10 +746,10 @@
         <v>7.5</v>
       </c>
       <c r="I9" t="n">
-        <v>54.88</v>
+        <v>55.47</v>
       </c>
       <c r="J9" t="n">
-        <v>7.41</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="10">
@@ -780,10 +780,10 @@
         <v>11.47</v>
       </c>
       <c r="I10" t="n">
-        <v>128.46</v>
+        <v>124.36</v>
       </c>
       <c r="J10" t="n">
-        <v>11.33</v>
+        <v>11.15</v>
       </c>
     </row>
     <row r="11">
@@ -814,10 +814,10 @@
         <v>11.47</v>
       </c>
       <c r="I11" t="n">
-        <v>199.09</v>
+        <v>148.66</v>
       </c>
       <c r="J11" t="n">
-        <v>14.11</v>
+        <v>12.19</v>
       </c>
     </row>
     <row r="12">
@@ -848,10 +848,10 @@
         <v>6.94</v>
       </c>
       <c r="I12" t="n">
-        <v>48.21</v>
+        <v>48.08</v>
       </c>
       <c r="J12" t="n">
-        <v>6.94</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="13">
@@ -882,10 +882,10 @@
         <v>6.94</v>
       </c>
       <c r="I13" t="n">
-        <v>48.66</v>
+        <v>48.26</v>
       </c>
       <c r="J13" t="n">
-        <v>6.98</v>
+        <v>6.95</v>
       </c>
     </row>
     <row r="14">
@@ -916,10 +916,10 @@
         <v>16.56</v>
       </c>
       <c r="I14" t="n">
-        <v>118.79</v>
+        <v>181.07</v>
       </c>
       <c r="J14" t="n">
-        <v>10.9</v>
+        <v>13.46</v>
       </c>
     </row>
     <row r="15">
@@ -950,10 +950,10 @@
         <v>16.56</v>
       </c>
       <c r="I15" t="n">
-        <v>1056.83</v>
+        <v>450.87</v>
       </c>
       <c r="J15" t="n">
-        <v>32.51</v>
+        <v>21.23</v>
       </c>
     </row>
     <row r="16">
@@ -984,10 +984,10 @@
         <v>23.06</v>
       </c>
       <c r="I16" t="n">
-        <v>100.21</v>
+        <v>211.08</v>
       </c>
       <c r="J16" t="n">
-        <v>10.01</v>
+        <v>14.53</v>
       </c>
     </row>
     <row r="17">
@@ -1018,10 +1018,10 @@
         <v>23.06</v>
       </c>
       <c r="I17" t="n">
-        <v>13584.26</v>
+        <v>1740.25</v>
       </c>
       <c r="J17" t="n">
-        <v>116.55</v>
+        <v>41.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(clinical-data): increase model error magnitudes for zone differentiation
- Increase error magnitudes 2-4x across all 8 clinical scenarios (A-H)
- Cap error magnitudes to ensure identical RMSE/MAE between Model A and B
- Maintain boundary controls (predictions >= 1 mg/dL)
- Zone A percentages reduced from ~100% to 0-43%
- Model B now shows Zone D classifications in critical scenarios
- Archive OpenSpec change increase-model-error-magnitude
</commit_message>
<xml_diff>
--- a/extended_outcome/extended_scenario_results.xlsx
+++ b/extended_outcome/extended_scenario_results.xlsx
@@ -487,31 +487,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>124.72</v>
+        <v>690.36</v>
       </c>
       <c r="H2" t="n">
-        <v>11.17</v>
+        <v>26.27</v>
       </c>
       <c r="I2" t="n">
-        <v>92.78</v>
+        <v>345.52</v>
       </c>
       <c r="J2" t="n">
-        <v>9.630000000000001</v>
+        <v>18.59</v>
       </c>
     </row>
     <row r="3">
@@ -521,31 +521,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>124.72</v>
+        <v>690.36</v>
       </c>
       <c r="H3" t="n">
-        <v>11.17</v>
+        <v>26.27</v>
       </c>
       <c r="I3" t="n">
-        <v>171.28</v>
+        <v>1592.76</v>
       </c>
       <c r="J3" t="n">
-        <v>13.09</v>
+        <v>39.91</v>
       </c>
     </row>
     <row r="4">
@@ -555,11 +555,11 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>50</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
@@ -570,16 +570,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>306.55</v>
+        <v>3616.35</v>
       </c>
       <c r="H4" t="n">
-        <v>17.51</v>
+        <v>60.14</v>
       </c>
       <c r="I4" t="n">
-        <v>171.31</v>
+        <v>666.85</v>
       </c>
       <c r="J4" t="n">
-        <v>13.09</v>
+        <v>25.82</v>
       </c>
     </row>
     <row r="5">
@@ -589,11 +589,11 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
         <v>50</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
@@ -604,16 +604,16 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>306.55</v>
+        <v>3616.35</v>
       </c>
       <c r="H5" t="n">
-        <v>17.51</v>
+        <v>60.14</v>
       </c>
       <c r="I5" t="n">
-        <v>600.1799999999999</v>
+        <v>79562.59</v>
       </c>
       <c r="J5" t="n">
-        <v>24.5</v>
+        <v>282.07</v>
       </c>
     </row>
     <row r="6">
@@ -623,11 +623,11 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
         <v>50</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
@@ -638,16 +638,16 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>95.59</v>
+        <v>1467.76</v>
       </c>
       <c r="H6" t="n">
-        <v>9.779999999999999</v>
+        <v>38.31</v>
       </c>
       <c r="I6" t="n">
-        <v>83.16</v>
+        <v>1205.76</v>
       </c>
       <c r="J6" t="n">
-        <v>9.119999999999999</v>
+        <v>34.72</v>
       </c>
     </row>
     <row r="7">
@@ -657,11 +657,11 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
         <v>50</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
@@ -672,16 +672,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>95.59</v>
+        <v>1467.76</v>
       </c>
       <c r="H7" t="n">
-        <v>9.779999999999999</v>
+        <v>38.31</v>
       </c>
       <c r="I7" t="n">
-        <v>113.81</v>
+        <v>5100.4</v>
       </c>
       <c r="J7" t="n">
-        <v>10.67</v>
+        <v>71.42</v>
       </c>
     </row>
     <row r="8">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -706,16 +706,16 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>56.23</v>
+        <v>881.96</v>
       </c>
       <c r="H8" t="n">
-        <v>7.5</v>
+        <v>29.7</v>
       </c>
       <c r="I8" t="n">
-        <v>57.28</v>
+        <v>1061.42</v>
       </c>
       <c r="J8" t="n">
-        <v>7.57</v>
+        <v>32.58</v>
       </c>
     </row>
     <row r="9">
@@ -725,10 +725,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -740,16 +740,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>56.23</v>
+        <v>881.96</v>
       </c>
       <c r="H9" t="n">
-        <v>7.5</v>
+        <v>29.7</v>
       </c>
       <c r="I9" t="n">
-        <v>55.47</v>
+        <v>891.16</v>
       </c>
       <c r="J9" t="n">
-        <v>7.45</v>
+        <v>29.85</v>
       </c>
     </row>
     <row r="10">
@@ -759,10 +759,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -774,16 +774,16 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>131.65</v>
+        <v>1401.05</v>
       </c>
       <c r="H10" t="n">
-        <v>11.47</v>
+        <v>37.43</v>
       </c>
       <c r="I10" t="n">
-        <v>124.36</v>
+        <v>1681.85</v>
       </c>
       <c r="J10" t="n">
-        <v>11.15</v>
+        <v>41.01</v>
       </c>
     </row>
     <row r="11">
@@ -793,10 +793,10 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
         <v>42</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -808,16 +808,16 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>131.65</v>
+        <v>1401.05</v>
       </c>
       <c r="H11" t="n">
-        <v>11.47</v>
+        <v>37.43</v>
       </c>
       <c r="I11" t="n">
-        <v>148.66</v>
+        <v>2323.89</v>
       </c>
       <c r="J11" t="n">
-        <v>12.19</v>
+        <v>48.21</v>
       </c>
     </row>
     <row r="12">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -842,16 +842,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>48.12</v>
+        <v>1069.76</v>
       </c>
       <c r="H12" t="n">
-        <v>6.94</v>
+        <v>32.71</v>
       </c>
       <c r="I12" t="n">
-        <v>48.08</v>
+        <v>1128.88</v>
       </c>
       <c r="J12" t="n">
-        <v>6.93</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="13">
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -876,16 +876,16 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>48.12</v>
+        <v>1069.76</v>
       </c>
       <c r="H13" t="n">
-        <v>6.94</v>
+        <v>32.71</v>
       </c>
       <c r="I13" t="n">
-        <v>48.26</v>
+        <v>1166.15</v>
       </c>
       <c r="J13" t="n">
-        <v>6.95</v>
+        <v>34.15</v>
       </c>
     </row>
     <row r="14">
@@ -895,10 +895,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -910,16 +910,16 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>274.29</v>
+        <v>2363.76</v>
       </c>
       <c r="H14" t="n">
-        <v>16.56</v>
+        <v>48.62</v>
       </c>
       <c r="I14" t="n">
-        <v>181.07</v>
+        <v>1092.52</v>
       </c>
       <c r="J14" t="n">
-        <v>13.46</v>
+        <v>33.05</v>
       </c>
     </row>
     <row r="15">
@@ -929,31 +929,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>274.29</v>
+        <v>2363.76</v>
       </c>
       <c r="H15" t="n">
-        <v>16.56</v>
+        <v>48.62</v>
       </c>
       <c r="I15" t="n">
-        <v>450.87</v>
+        <v>23847.39</v>
       </c>
       <c r="J15" t="n">
-        <v>21.23</v>
+        <v>154.43</v>
       </c>
     </row>
     <row r="16">
@@ -963,10 +963,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>531.76</v>
+        <v>3928.49</v>
       </c>
       <c r="H16" t="n">
-        <v>23.06</v>
+        <v>62.68</v>
       </c>
       <c r="I16" t="n">
-        <v>211.08</v>
+        <v>805.8200000000001</v>
       </c>
       <c r="J16" t="n">
-        <v>14.53</v>
+        <v>28.39</v>
       </c>
     </row>
     <row r="17">
@@ -997,31 +997,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>531.76</v>
+        <v>3928.49</v>
       </c>
       <c r="H17" t="n">
-        <v>23.06</v>
+        <v>62.68</v>
       </c>
       <c r="I17" t="n">
-        <v>1740.25</v>
+        <v>302771.23</v>
       </c>
       <c r="J17" t="n">
-        <v>41.72</v>
+        <v>550.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(clinical-data): add random variance to predictions and improve timeseries
- Add random variance (±0-15 mg/dL) to model prediction errors
- Variance applied to error magnitude to maintain equal RMSE/MAE between models
- Timeseries plots now only show predictions outside euglycemic range (70-180)
- Use np.nan masking to hide predictions in normal glucose range
- Archive OpenSpec change add-prediction-variance
</commit_message>
<xml_diff>
--- a/extended_outcome/extended_scenario_results.xlsx
+++ b/extended_outcome/extended_scenario_results.xlsx
@@ -487,31 +487,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>690.36</v>
+        <v>668.34</v>
       </c>
       <c r="H2" t="n">
-        <v>26.27</v>
+        <v>25.85</v>
       </c>
       <c r="I2" t="n">
-        <v>345.52</v>
+        <v>288.4</v>
       </c>
       <c r="J2" t="n">
-        <v>18.59</v>
+        <v>16.98</v>
       </c>
     </row>
     <row r="3">
@@ -521,31 +521,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>690.36</v>
+        <v>668.34</v>
       </c>
       <c r="H3" t="n">
-        <v>26.27</v>
+        <v>25.85</v>
       </c>
       <c r="I3" t="n">
-        <v>1592.76</v>
+        <v>1745.32</v>
       </c>
       <c r="J3" t="n">
-        <v>39.91</v>
+        <v>41.78</v>
       </c>
     </row>
     <row r="4">
@@ -555,10 +555,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -570,16 +570,16 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>3616.35</v>
+        <v>3451.83</v>
       </c>
       <c r="H4" t="n">
-        <v>60.14</v>
+        <v>58.75</v>
       </c>
       <c r="I4" t="n">
-        <v>666.85</v>
+        <v>697.62</v>
       </c>
       <c r="J4" t="n">
-        <v>25.82</v>
+        <v>26.41</v>
       </c>
     </row>
     <row r="5">
@@ -589,31 +589,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>3616.35</v>
+        <v>3451.83</v>
       </c>
       <c r="H5" t="n">
-        <v>60.14</v>
+        <v>58.75</v>
       </c>
       <c r="I5" t="n">
-        <v>79562.59</v>
+        <v>62074.86</v>
       </c>
       <c r="J5" t="n">
-        <v>282.07</v>
+        <v>249.15</v>
       </c>
     </row>
     <row r="6">
@@ -623,10 +623,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -638,16 +638,16 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1467.76</v>
+        <v>1474.42</v>
       </c>
       <c r="H6" t="n">
-        <v>38.31</v>
+        <v>38.4</v>
       </c>
       <c r="I6" t="n">
-        <v>1205.76</v>
+        <v>1046.78</v>
       </c>
       <c r="J6" t="n">
-        <v>34.72</v>
+        <v>32.35</v>
       </c>
     </row>
     <row r="7">
@@ -657,10 +657,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -672,16 +672,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1467.76</v>
+        <v>1474.42</v>
       </c>
       <c r="H7" t="n">
-        <v>38.31</v>
+        <v>38.4</v>
       </c>
       <c r="I7" t="n">
-        <v>5100.4</v>
+        <v>6599.73</v>
       </c>
       <c r="J7" t="n">
-        <v>71.42</v>
+        <v>81.23999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -706,16 +706,16 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>881.96</v>
+        <v>977.9400000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>29.7</v>
+        <v>31.27</v>
       </c>
       <c r="I8" t="n">
-        <v>1061.42</v>
+        <v>1096.54</v>
       </c>
       <c r="J8" t="n">
-        <v>32.58</v>
+        <v>33.11</v>
       </c>
     </row>
     <row r="9">
@@ -725,10 +725,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -740,16 +740,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>881.96</v>
+        <v>977.9400000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>29.7</v>
+        <v>31.27</v>
       </c>
       <c r="I9" t="n">
-        <v>891.16</v>
+        <v>1133.86</v>
       </c>
       <c r="J9" t="n">
-        <v>29.85</v>
+        <v>33.67</v>
       </c>
     </row>
     <row r="10">
@@ -759,31 +759,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1401.05</v>
+        <v>1428.7</v>
       </c>
       <c r="H10" t="n">
-        <v>37.43</v>
+        <v>37.8</v>
       </c>
       <c r="I10" t="n">
-        <v>1681.85</v>
+        <v>1392.81</v>
       </c>
       <c r="J10" t="n">
-        <v>41.01</v>
+        <v>37.32</v>
       </c>
     </row>
     <row r="11">
@@ -793,31 +793,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1401.05</v>
+        <v>1428.7</v>
       </c>
       <c r="H11" t="n">
-        <v>37.43</v>
+        <v>37.8</v>
       </c>
       <c r="I11" t="n">
-        <v>2323.89</v>
+        <v>2998.31</v>
       </c>
       <c r="J11" t="n">
-        <v>48.21</v>
+        <v>54.76</v>
       </c>
     </row>
     <row r="12">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -842,16 +842,16 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>1069.76</v>
+        <v>1255.72</v>
       </c>
       <c r="H12" t="n">
-        <v>32.71</v>
+        <v>35.44</v>
       </c>
       <c r="I12" t="n">
-        <v>1128.88</v>
+        <v>1329.54</v>
       </c>
       <c r="J12" t="n">
-        <v>33.6</v>
+        <v>36.46</v>
       </c>
     </row>
     <row r="13">
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -876,16 +876,16 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1069.76</v>
+        <v>1255.72</v>
       </c>
       <c r="H13" t="n">
-        <v>32.71</v>
+        <v>35.44</v>
       </c>
       <c r="I13" t="n">
-        <v>1166.15</v>
+        <v>1465.81</v>
       </c>
       <c r="J13" t="n">
-        <v>34.15</v>
+        <v>38.29</v>
       </c>
     </row>
     <row r="14">
@@ -895,10 +895,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -910,16 +910,16 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>2363.76</v>
+        <v>2427.07</v>
       </c>
       <c r="H14" t="n">
-        <v>48.62</v>
+        <v>49.27</v>
       </c>
       <c r="I14" t="n">
-        <v>1092.52</v>
+        <v>1450.36</v>
       </c>
       <c r="J14" t="n">
-        <v>33.05</v>
+        <v>38.08</v>
       </c>
     </row>
     <row r="15">
@@ -929,31 +929,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>2363.76</v>
+        <v>2427.07</v>
       </c>
       <c r="H15" t="n">
-        <v>48.62</v>
+        <v>49.27</v>
       </c>
       <c r="I15" t="n">
-        <v>23847.39</v>
+        <v>25283.48</v>
       </c>
       <c r="J15" t="n">
-        <v>154.43</v>
+        <v>159.01</v>
       </c>
     </row>
     <row r="16">
@@ -963,10 +963,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>3928.49</v>
+        <v>3960.2</v>
       </c>
       <c r="H16" t="n">
-        <v>62.68</v>
+        <v>62.93</v>
       </c>
       <c r="I16" t="n">
-        <v>805.8200000000001</v>
+        <v>775.91</v>
       </c>
       <c r="J16" t="n">
-        <v>28.39</v>
+        <v>27.86</v>
       </c>
     </row>
     <row r="17">
@@ -997,10 +997,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1012,16 +1012,16 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>3928.49</v>
+        <v>3960.2</v>
       </c>
       <c r="H17" t="n">
-        <v>62.68</v>
+        <v>62.93</v>
       </c>
       <c r="I17" t="n">
-        <v>302771.23</v>
+        <v>349556.81</v>
       </c>
       <c r="J17" t="n">
-        <v>550.25</v>
+        <v>591.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>